<commit_message>
Remove Web & Update README.md
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11056\Desktop\Research\caltable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4715513C-D63C-4EBB-8D74-36C6E61C2E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973001AA-8B3D-401E-93DB-F035B3465724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="4040" windowWidth="14400" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>6cdb</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,6 +53,9 @@
   <si>
     <t>montecarlo</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sconf_weight</t>
   </si>
 </sst>
 </file>
@@ -377,23 +380,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -403,8 +409,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -413,10 +422,14 @@
       </c>
       <c r="C3" t="s">
         <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>